<commit_message>
last month data logic updated
</commit_message>
<xml_diff>
--- a/BillAppDocs/OnceConfigureData.xlsx
+++ b/BillAppDocs/OnceConfigureData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDir\Walee\Backup\ShortCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDir\Walee\Bill-Website-Walee\BillAppDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA88DA52-4293-4B74-9E88-5B2B04B242B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBEA6F8-EF01-495B-9D95-2C2E58A30091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BS2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="BB7" sqref="BB7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>